<commit_message>
up to what before 考察
</commit_message>
<xml_diff>
--- a/状態図.xlsx
+++ b/状態図.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoshi\Documents\物理実験2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoshi\Documents\物理実験2\reportFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA2501C-C261-4FCC-84EF-245F93A1FC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65173C4A-FBC0-4499-A4C3-FB5A8A19FC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4CE216AB-8ED5-4123-BC20-9E9DBB3BBEF1}"/>
   </bookViews>
@@ -36,14 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Snの割合</t>
-    <rPh sb="3" eb="5">
-      <t>ワリアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>温度（固相線）</t>
     <rPh sb="0" eb="2">
@@ -52,6 +45,18 @@
     <rPh sb="3" eb="6">
       <t>コソウセン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>solid phase line</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>liquid phase line</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ratio of Sn</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -134,6 +139,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>状態図</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -172,10 +203,15 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>固相線</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="82000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -266,6 +302,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>液相線</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1496,23 +1535,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA94DF3-B291-43E9-B4A5-45C308F0F1A4}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1520,7 +1563,7 @@
         <v>418.77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1531,7 +1574,7 @@
         <v>360.11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1542,7 +1585,7 @@
         <v>318.67</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1553,7 +1596,7 @@
         <v>291.92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>7</v>
       </c>
@@ -1564,7 +1607,7 @@
         <v>220.87</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>8.5</v>
       </c>
@@ -1575,7 +1618,7 @@
         <v>201.75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1586,7 +1629,7 @@
         <v>231.14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>10</v>
       </c>

</xml_diff>